<commit_message>
feat: add lethality table
</commit_message>
<xml_diff>
--- a/tables/tables_presentation.xlsx
+++ b/tables/tables_presentation.xlsx
@@ -12,6 +12,8 @@
     <sheet name="Regions" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Race" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Hospitals" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lethality Region" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Lethality Hospital" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="28">
   <si>
     <t xml:space="preserve">Data Information</t>
   </si>
@@ -101,19 +103,31 @@
     <t xml:space="preserve">Private</t>
   </si>
   <si>
-    <t xml:space="preserve">ONG</t>
+    <t xml:space="preserve">Philanthropic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age-adjusted In-hospital
+Lethality rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age-adjusted ICU
+Lethality rate*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]#,##0"/>
     <numFmt numFmtId="166" formatCode="[$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
+    <numFmt numFmtId="168" formatCode="[$-409]General"/>
+    <numFmt numFmtId="169" formatCode="[$-409]@"/>
+    <numFmt numFmtId="170" formatCode="[$-409]0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,6 +162,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,7 +268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,6 +381,46 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,13 +440,14 @@
   </sheetPr>
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="0" width="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,15 +1062,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="0" width="10.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,6 +2191,9 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2148,13 +2213,14 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="0" width="11.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,15 +2915,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="0" width="11.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3272,6 +3339,89 @@
       <c r="M10" s="0"/>
       <c r="N10" s="0"/>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="30"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="31"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3281,4 +3431,1036 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G1" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="J1" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>0.06585</v>
+      </c>
+      <c r="C2" s="32" t="n">
+        <v>0.07017</v>
+      </c>
+      <c r="D2" s="32" t="n">
+        <v>0.07309</v>
+      </c>
+      <c r="E2" s="32" t="n">
+        <v>0.07387</v>
+      </c>
+      <c r="F2" s="32" t="n">
+        <v>0.07981</v>
+      </c>
+      <c r="G2" s="32" t="n">
+        <v>0.08658</v>
+      </c>
+      <c r="H2" s="32" t="n">
+        <v>0.08191</v>
+      </c>
+      <c r="I2" s="32" t="n">
+        <v>0.0858</v>
+      </c>
+      <c r="J2" s="32" t="n">
+        <v>0.08662</v>
+      </c>
+      <c r="K2" s="15" t="n">
+        <v>31.5413819286257</v>
+      </c>
+      <c r="L2" s="15" t="n">
+        <v>3.48343473343751</v>
+      </c>
+      <c r="M2" s="15" t="n">
+        <v>3.28842002005567</v>
+      </c>
+      <c r="N2" s="16" t="n">
+        <v>3.67881764625957</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="33" t="n">
+        <v>0.05104</v>
+      </c>
+      <c r="C3" s="33" t="n">
+        <v>0.05767</v>
+      </c>
+      <c r="D3" s="33" t="n">
+        <v>0.05853</v>
+      </c>
+      <c r="E3" s="33" t="n">
+        <v>0.06312</v>
+      </c>
+      <c r="F3" s="33" t="n">
+        <v>0.06221</v>
+      </c>
+      <c r="G3" s="33" t="n">
+        <v>0.06203</v>
+      </c>
+      <c r="H3" s="33" t="n">
+        <v>0.05907</v>
+      </c>
+      <c r="I3" s="33" t="n">
+        <v>0.06313</v>
+      </c>
+      <c r="J3" s="33" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="K3" s="18" t="n">
+        <v>29.3103448275862</v>
+      </c>
+      <c r="L3" s="18" t="n">
+        <v>2.14654213726213</v>
+      </c>
+      <c r="M3" s="18" t="n">
+        <v>1.69362271805456</v>
+      </c>
+      <c r="N3" s="19" t="n">
+        <v>2.6014787527777</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="33" t="n">
+        <v>0.04194</v>
+      </c>
+      <c r="C4" s="33" t="n">
+        <v>0.04628</v>
+      </c>
+      <c r="D4" s="33" t="n">
+        <v>0.04551</v>
+      </c>
+      <c r="E4" s="33" t="n">
+        <v>0.05242</v>
+      </c>
+      <c r="F4" s="33" t="n">
+        <v>0.06046</v>
+      </c>
+      <c r="G4" s="33" t="n">
+        <v>0.07225</v>
+      </c>
+      <c r="H4" s="33" t="n">
+        <v>0.0674</v>
+      </c>
+      <c r="I4" s="33" t="n">
+        <v>0.07232</v>
+      </c>
+      <c r="J4" s="33" t="n">
+        <v>0.07491</v>
+      </c>
+      <c r="K4" s="18" t="n">
+        <v>78.6123032904149</v>
+      </c>
+      <c r="L4" s="18" t="n">
+        <v>8.05593902482411</v>
+      </c>
+      <c r="M4" s="18" t="n">
+        <v>7.17677757552724</v>
+      </c>
+      <c r="N4" s="19" t="n">
+        <v>8.94231215627281</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="33" t="n">
+        <v>0.04194</v>
+      </c>
+      <c r="C5" s="33" t="n">
+        <v>0.04628</v>
+      </c>
+      <c r="D5" s="33" t="n">
+        <v>0.04551</v>
+      </c>
+      <c r="E5" s="33" t="n">
+        <v>0.05242</v>
+      </c>
+      <c r="F5" s="33" t="n">
+        <v>0.06046</v>
+      </c>
+      <c r="G5" s="33" t="n">
+        <v>0.07225</v>
+      </c>
+      <c r="H5" s="33" t="n">
+        <v>0.0674</v>
+      </c>
+      <c r="I5" s="33" t="n">
+        <v>0.07232</v>
+      </c>
+      <c r="J5" s="33" t="n">
+        <v>0.07491</v>
+      </c>
+      <c r="K5" s="18" t="n">
+        <v>78.6123032904149</v>
+      </c>
+      <c r="L5" s="18" t="n">
+        <v>8.05593902482411</v>
+      </c>
+      <c r="M5" s="18" t="n">
+        <v>7.17677757552724</v>
+      </c>
+      <c r="N5" s="19" t="n">
+        <v>8.94231215627281</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="33" t="n">
+        <v>0.09784</v>
+      </c>
+      <c r="C6" s="33" t="n">
+        <v>0.09908</v>
+      </c>
+      <c r="D6" s="33" t="n">
+        <v>0.0997</v>
+      </c>
+      <c r="E6" s="33" t="n">
+        <v>0.09611</v>
+      </c>
+      <c r="F6" s="33" t="n">
+        <v>0.10689</v>
+      </c>
+      <c r="G6" s="33" t="n">
+        <v>0.10765</v>
+      </c>
+      <c r="H6" s="33" t="n">
+        <v>0.10297</v>
+      </c>
+      <c r="I6" s="33" t="n">
+        <v>0.11096</v>
+      </c>
+      <c r="J6" s="33" t="n">
+        <v>0.10835</v>
+      </c>
+      <c r="K6" s="18" t="n">
+        <v>10.7420278004906</v>
+      </c>
+      <c r="L6" s="18" t="n">
+        <v>1.55247811276245</v>
+      </c>
+      <c r="M6" s="18" t="n">
+        <v>1.2828345260675</v>
+      </c>
+      <c r="N6" s="19" t="n">
+        <v>1.82283956704259</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="33" t="n">
+        <v>0.05819</v>
+      </c>
+      <c r="C7" s="33" t="n">
+        <v>0.0587</v>
+      </c>
+      <c r="D7" s="33" t="n">
+        <v>0.06286</v>
+      </c>
+      <c r="E7" s="33" t="n">
+        <v>0.06484</v>
+      </c>
+      <c r="F7" s="33" t="n">
+        <v>0.07322</v>
+      </c>
+      <c r="G7" s="33" t="n">
+        <v>0.0817</v>
+      </c>
+      <c r="H7" s="33" t="n">
+        <v>0.07749</v>
+      </c>
+      <c r="I7" s="33" t="n">
+        <v>0.08232</v>
+      </c>
+      <c r="J7" s="33" t="n">
+        <v>0.08237</v>
+      </c>
+      <c r="K7" s="18" t="n">
+        <v>41.5535315346279</v>
+      </c>
+      <c r="L7" s="18" t="n">
+        <v>5.15357070525546</v>
+      </c>
+      <c r="M7" s="18" t="n">
+        <v>4.41854392534628</v>
+      </c>
+      <c r="N7" s="19" t="n">
+        <v>5.89377151218009</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="32" t="n">
+        <v>0.45356</v>
+      </c>
+      <c r="C8" s="32" t="n">
+        <v>0.44942</v>
+      </c>
+      <c r="D8" s="32" t="n">
+        <v>0.45464</v>
+      </c>
+      <c r="E8" s="32" t="n">
+        <v>0.45875</v>
+      </c>
+      <c r="F8" s="32" t="n">
+        <v>0.46619</v>
+      </c>
+      <c r="G8" s="32" t="n">
+        <v>0.45586</v>
+      </c>
+      <c r="H8" s="32" t="n">
+        <v>0.44215</v>
+      </c>
+      <c r="I8" s="32" t="n">
+        <v>0.44198</v>
+      </c>
+      <c r="J8" s="32" t="n">
+        <v>0.39867</v>
+      </c>
+      <c r="K8" s="15" t="n">
+        <v>-12.1020372166858</v>
+      </c>
+      <c r="L8" s="15" t="n">
+        <v>-1.11786064737655</v>
+      </c>
+      <c r="M8" s="15" t="n">
+        <v>-1.4542570625482</v>
+      </c>
+      <c r="N8" s="16" t="n">
+        <v>-0.780315907124907</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="33" t="n">
+        <v>0.42993</v>
+      </c>
+      <c r="C9" s="33" t="n">
+        <v>0.44698</v>
+      </c>
+      <c r="D9" s="33" t="n">
+        <v>0.42016</v>
+      </c>
+      <c r="E9" s="33" t="n">
+        <v>0.44043</v>
+      </c>
+      <c r="F9" s="33" t="n">
+        <v>0.43962</v>
+      </c>
+      <c r="G9" s="33" t="n">
+        <v>0.42673</v>
+      </c>
+      <c r="H9" s="33" t="n">
+        <v>0.38812</v>
+      </c>
+      <c r="I9" s="33" t="n">
+        <v>0.38736</v>
+      </c>
+      <c r="J9" s="33" t="n">
+        <v>0.34092</v>
+      </c>
+      <c r="K9" s="18" t="n">
+        <v>-20.703370316098</v>
+      </c>
+      <c r="L9" s="18" t="n">
+        <v>-2.61530732809823</v>
+      </c>
+      <c r="M9" s="18" t="n">
+        <v>-3.34289328692596</v>
+      </c>
+      <c r="N9" s="19" t="n">
+        <v>-1.88224446906641</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="33" t="n">
+        <v>0.51919</v>
+      </c>
+      <c r="C10" s="33" t="n">
+        <v>0.55848</v>
+      </c>
+      <c r="D10" s="33" t="n">
+        <v>0.57501</v>
+      </c>
+      <c r="E10" s="33" t="n">
+        <v>0.55261</v>
+      </c>
+      <c r="F10" s="33" t="n">
+        <v>0.58473</v>
+      </c>
+      <c r="G10" s="33" t="n">
+        <v>0.62401</v>
+      </c>
+      <c r="H10" s="33" t="n">
+        <v>0.56389</v>
+      </c>
+      <c r="I10" s="33" t="n">
+        <v>0.55673</v>
+      </c>
+      <c r="J10" s="33" t="n">
+        <v>0.51552</v>
+      </c>
+      <c r="K10" s="18" t="n">
+        <v>-0.706870317224908</v>
+      </c>
+      <c r="L10" s="18" t="n">
+        <v>-0.121084186207332</v>
+      </c>
+      <c r="M10" s="18" t="n">
+        <v>-1.6427753760723</v>
+      </c>
+      <c r="N10" s="19" t="n">
+        <v>1.42414918966549</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="33" t="n">
+        <v>0.51919</v>
+      </c>
+      <c r="C11" s="33" t="n">
+        <v>0.55848</v>
+      </c>
+      <c r="D11" s="33" t="n">
+        <v>0.57501</v>
+      </c>
+      <c r="E11" s="33" t="n">
+        <v>0.55261</v>
+      </c>
+      <c r="F11" s="33" t="n">
+        <v>0.58473</v>
+      </c>
+      <c r="G11" s="33" t="n">
+        <v>0.62401</v>
+      </c>
+      <c r="H11" s="33" t="n">
+        <v>0.56389</v>
+      </c>
+      <c r="I11" s="33" t="n">
+        <v>0.55673</v>
+      </c>
+      <c r="J11" s="33" t="n">
+        <v>0.51552</v>
+      </c>
+      <c r="K11" s="18" t="n">
+        <v>-0.706870317224908</v>
+      </c>
+      <c r="L11" s="18" t="n">
+        <v>-0.121084186207332</v>
+      </c>
+      <c r="M11" s="18" t="n">
+        <v>-1.6427753760723</v>
+      </c>
+      <c r="N11" s="19" t="n">
+        <v>1.42414918966549</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="33" t="n">
+        <v>0.44345</v>
+      </c>
+      <c r="C12" s="33" t="n">
+        <v>0.42419</v>
+      </c>
+      <c r="D12" s="33" t="n">
+        <v>0.40865</v>
+      </c>
+      <c r="E12" s="33" t="n">
+        <v>0.40972</v>
+      </c>
+      <c r="F12" s="33" t="n">
+        <v>0.43986</v>
+      </c>
+      <c r="G12" s="33" t="n">
+        <v>0.41672</v>
+      </c>
+      <c r="H12" s="33" t="n">
+        <v>0.41372</v>
+      </c>
+      <c r="I12" s="33" t="n">
+        <v>0.41631</v>
+      </c>
+      <c r="J12" s="33" t="n">
+        <v>0.37389</v>
+      </c>
+      <c r="K12" s="18" t="n">
+        <v>-15.6860976434773</v>
+      </c>
+      <c r="L12" s="18" t="n">
+        <v>-1.16715790996236</v>
+      </c>
+      <c r="M12" s="18" t="n">
+        <v>-1.67319841799506</v>
+      </c>
+      <c r="N12" s="19" t="n">
+        <v>-0.65851305609872</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="35" t="n">
+        <v>0.44638</v>
+      </c>
+      <c r="C13" s="35" t="n">
+        <v>0.40599</v>
+      </c>
+      <c r="D13" s="35" t="n">
+        <v>0.4877</v>
+      </c>
+      <c r="E13" s="35" t="n">
+        <v>0.43266</v>
+      </c>
+      <c r="F13" s="35" t="n">
+        <v>0.44297</v>
+      </c>
+      <c r="G13" s="35" t="n">
+        <v>0.45788</v>
+      </c>
+      <c r="H13" s="35" t="n">
+        <v>0.4024</v>
+      </c>
+      <c r="I13" s="35" t="n">
+        <v>0.47425</v>
+      </c>
+      <c r="J13" s="35" t="n">
+        <v>0.42259</v>
+      </c>
+      <c r="K13" s="22" t="n">
+        <v>-5.32953985393611</v>
+      </c>
+      <c r="L13" s="22" t="n">
+        <v>-0.203531665419065</v>
+      </c>
+      <c r="M13" s="22" t="n">
+        <v>-1.22142501744456</v>
+      </c>
+      <c r="N13" s="23" t="n">
+        <v>0.824850872913063</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G1" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="J1" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="32" t="n">
+        <v>0.06585</v>
+      </c>
+      <c r="C2" s="32" t="n">
+        <v>0.07017</v>
+      </c>
+      <c r="D2" s="32" t="n">
+        <v>0.07309</v>
+      </c>
+      <c r="E2" s="32" t="n">
+        <v>0.07387</v>
+      </c>
+      <c r="F2" s="32" t="n">
+        <v>0.07981</v>
+      </c>
+      <c r="G2" s="32" t="n">
+        <v>0.08658</v>
+      </c>
+      <c r="H2" s="32" t="n">
+        <v>0.08191</v>
+      </c>
+      <c r="I2" s="32" t="n">
+        <v>0.0858</v>
+      </c>
+      <c r="J2" s="32" t="n">
+        <v>0.08662</v>
+      </c>
+      <c r="K2" s="15" t="n">
+        <v>31.5413819286257</v>
+      </c>
+      <c r="L2" s="15" t="n">
+        <v>3.48343473343751</v>
+      </c>
+      <c r="M2" s="15" t="n">
+        <v>3.28842002005567</v>
+      </c>
+      <c r="N2" s="16" t="n">
+        <v>3.67881764625957</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="36" t="n">
+        <v>0.08268</v>
+      </c>
+      <c r="C3" s="36" t="n">
+        <v>0.0858</v>
+      </c>
+      <c r="D3" s="36" t="n">
+        <v>0.08682</v>
+      </c>
+      <c r="E3" s="36" t="n">
+        <v>0.08737</v>
+      </c>
+      <c r="F3" s="36" t="n">
+        <v>0.09678</v>
+      </c>
+      <c r="G3" s="36" t="n">
+        <v>0.1085</v>
+      </c>
+      <c r="H3" s="36" t="n">
+        <v>0.0997</v>
+      </c>
+      <c r="I3" s="36" t="n">
+        <v>0.10279</v>
+      </c>
+      <c r="J3" s="36" t="n">
+        <v>0.10134</v>
+      </c>
+      <c r="K3" s="11" t="n">
+        <v>22.5689404934688</v>
+      </c>
+      <c r="L3" s="11" t="n">
+        <v>3.04882322072166</v>
+      </c>
+      <c r="M3" s="11" t="n">
+        <v>2.77825387131414</v>
+      </c>
+      <c r="N3" s="12" t="n">
+        <v>3.32010485867353</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="36" t="n">
+        <v>0.02895</v>
+      </c>
+      <c r="C4" s="36" t="n">
+        <v>0.03111</v>
+      </c>
+      <c r="D4" s="36" t="n">
+        <v>0.04054</v>
+      </c>
+      <c r="E4" s="36" t="n">
+        <v>0.03963</v>
+      </c>
+      <c r="F4" s="36" t="n">
+        <v>0.03769</v>
+      </c>
+      <c r="G4" s="36" t="n">
+        <v>0.04659</v>
+      </c>
+      <c r="H4" s="36" t="n">
+        <v>0.03765</v>
+      </c>
+      <c r="I4" s="36" t="n">
+        <v>0.03801</v>
+      </c>
+      <c r="J4" s="36" t="n">
+        <v>0.0378</v>
+      </c>
+      <c r="K4" s="11" t="n">
+        <v>30.5699481865285</v>
+      </c>
+      <c r="L4" s="11" t="n">
+        <v>2.74898117422206</v>
+      </c>
+      <c r="M4" s="11" t="n">
+        <v>1.69921606750252</v>
+      </c>
+      <c r="N4" s="12" t="n">
+        <v>3.80958222267151</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="36" t="n">
+        <v>0.06595</v>
+      </c>
+      <c r="C5" s="36" t="n">
+        <v>0.07189</v>
+      </c>
+      <c r="D5" s="36" t="n">
+        <v>0.07212</v>
+      </c>
+      <c r="E5" s="36" t="n">
+        <v>0.07372</v>
+      </c>
+      <c r="F5" s="36" t="n">
+        <v>0.07755</v>
+      </c>
+      <c r="G5" s="36" t="n">
+        <v>0.0789</v>
+      </c>
+      <c r="H5" s="36" t="n">
+        <v>0.07552</v>
+      </c>
+      <c r="I5" s="36" t="n">
+        <v>0.07873</v>
+      </c>
+      <c r="J5" s="36" t="n">
+        <v>0.08225</v>
+      </c>
+      <c r="K5" s="11" t="n">
+        <v>24.7156937073541</v>
+      </c>
+      <c r="L5" s="11" t="n">
+        <v>2.18357813426757</v>
+      </c>
+      <c r="M5" s="11" t="n">
+        <v>1.89507261369994</v>
+      </c>
+      <c r="N5" s="12" t="n">
+        <v>2.47290052883371</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="32" t="n">
+        <v>0.45356</v>
+      </c>
+      <c r="C6" s="32" t="n">
+        <v>0.44942</v>
+      </c>
+      <c r="D6" s="32" t="n">
+        <v>0.45464</v>
+      </c>
+      <c r="E6" s="32" t="n">
+        <v>0.45875</v>
+      </c>
+      <c r="F6" s="32" t="n">
+        <v>0.46619</v>
+      </c>
+      <c r="G6" s="32" t="n">
+        <v>0.45586</v>
+      </c>
+      <c r="H6" s="32" t="n">
+        <v>0.44215</v>
+      </c>
+      <c r="I6" s="32" t="n">
+        <v>0.44198</v>
+      </c>
+      <c r="J6" s="32" t="n">
+        <v>0.39867</v>
+      </c>
+      <c r="K6" s="15" t="n">
+        <v>-12.1020372166858</v>
+      </c>
+      <c r="L6" s="15" t="n">
+        <v>-1.11786064737655</v>
+      </c>
+      <c r="M6" s="15" t="n">
+        <v>-1.4542570625482</v>
+      </c>
+      <c r="N6" s="16" t="n">
+        <v>-0.780315907124907</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="36" t="n">
+        <v>0.47779</v>
+      </c>
+      <c r="C7" s="36" t="n">
+        <v>0.46235</v>
+      </c>
+      <c r="D7" s="36" t="n">
+        <v>0.47575</v>
+      </c>
+      <c r="E7" s="36" t="n">
+        <v>0.47575</v>
+      </c>
+      <c r="F7" s="36" t="n">
+        <v>0.47849</v>
+      </c>
+      <c r="G7" s="36" t="n">
+        <v>0.46512</v>
+      </c>
+      <c r="H7" s="36" t="n">
+        <v>0.4734</v>
+      </c>
+      <c r="I7" s="36" t="n">
+        <v>0.47453</v>
+      </c>
+      <c r="J7" s="36" t="n">
+        <v>0.41213</v>
+      </c>
+      <c r="K7" s="11" t="n">
+        <v>-13.7424391469055</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>-1.00580139418204</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>-1.58520674318323</v>
+      </c>
+      <c r="N7" s="12" t="n">
+        <v>-0.422984865343534</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="36" t="n">
+        <v>0.34814</v>
+      </c>
+      <c r="C8" s="36" t="n">
+        <v>0.33271</v>
+      </c>
+      <c r="D8" s="36" t="n">
+        <v>0.41639</v>
+      </c>
+      <c r="E8" s="36" t="n">
+        <v>0.39092</v>
+      </c>
+      <c r="F8" s="36" t="n">
+        <v>0.39166</v>
+      </c>
+      <c r="G8" s="36" t="n">
+        <v>0.45638</v>
+      </c>
+      <c r="H8" s="36" t="n">
+        <v>0.37288</v>
+      </c>
+      <c r="I8" s="36" t="n">
+        <v>0.38449</v>
+      </c>
+      <c r="J8" s="36" t="n">
+        <v>0.33585</v>
+      </c>
+      <c r="K8" s="11" t="n">
+        <v>-3.53018900442351</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>-0.132956018550356</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>-1.35478661265062</v>
+      </c>
+      <c r="N8" s="12" t="n">
+        <v>1.10400830530135</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="37" t="n">
+        <v>0.45609</v>
+      </c>
+      <c r="C9" s="37" t="n">
+        <v>0.46132</v>
+      </c>
+      <c r="D9" s="37" t="n">
+        <v>0.44986</v>
+      </c>
+      <c r="E9" s="37" t="n">
+        <v>0.46169</v>
+      </c>
+      <c r="F9" s="37" t="n">
+        <v>0.47155</v>
+      </c>
+      <c r="G9" s="37" t="n">
+        <v>0.45164</v>
+      </c>
+      <c r="H9" s="37" t="n">
+        <v>0.43261</v>
+      </c>
+      <c r="I9" s="37" t="n">
+        <v>0.42591</v>
+      </c>
+      <c r="J9" s="37" t="n">
+        <v>0.40155</v>
+      </c>
+      <c r="K9" s="26" t="n">
+        <v>-11.9581661514175</v>
+      </c>
+      <c r="L9" s="26" t="n">
+        <v>-1.46897302641714</v>
+      </c>
+      <c r="M9" s="26" t="n">
+        <v>-1.91841440417102</v>
+      </c>
+      <c r="N9" s="27" t="n">
+        <v>-1.01747216368644</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>